<commit_message>
remove variance bias, linear variance, calc cost
</commit_message>
<xml_diff>
--- a/ToolBox/MomentumFactor.xlsx
+++ b/ToolBox/MomentumFactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cheng\Documents\Proj\VarianceArithemtic\ToolBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E77DEC-C6F3-49C7-9110-44CAB6F3DEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7415DC28-0257-479F-8CC0-B0DBA4F883FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FD3F55C-C7F1-40E3-A8ED-B74ABB74A617}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{7FD3F55C-C7F1-40E3-A8ED-B74ABB74A617}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>s</t>
   </si>
@@ -50,30 +50,6 @@
   </si>
   <si>
     <t>Leakage</t>
-  </si>
-  <si>
-    <t>P(x)</t>
-  </si>
-  <si>
-    <t>SQ</t>
-  </si>
-  <si>
-    <t>SQRT</t>
-  </si>
-  <si>
-    <t>Dev</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Cost/Linear</t>
-  </si>
-  <si>
-    <t>Linear</t>
-  </si>
-  <si>
-    <t>Dev/2</t>
   </si>
 </sst>
 </file>
@@ -16129,7 +16105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69331D1-8607-4904-B05A-525081DDFA9E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
@@ -41209,10 +41185,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3291F485-E684-4872-B375-DA358E51D423}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41221,30 +41197,15 @@
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1">
-        <v>4</v>
-      </c>
-      <c r="I1">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3</v>
       </c>
@@ -41252,303 +41213,66 @@
         <f>1-ERF(A2/SQRT(2))</f>
         <v>2.6997960632602069E-3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <f>1/E1</f>
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:I2" si="0">1/F1</f>
-        <v>0.5</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H2">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="I2">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" si="1">1-ERF(A3/SQRT(2))</f>
+        <f t="shared" ref="B3:B6" si="0">1-ERF(A3/SQRT(2))</f>
         <v>6.3342483666239957E-5</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <f>E2*2</f>
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:I3" si="2">F2*2</f>
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="2"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.7330314373604807E-7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <f>SQRT(4*E2+2*E2^2)</f>
-        <v>2.4494897427831779</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:I4" si="3">SQRT(4*F2+2*F2^2)</f>
-        <v>1.5811388300841898</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="3"/>
-        <v>1.247219128924647</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="3"/>
-        <v>1.0606601717798212</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="3"/>
-        <v>0.93808315196468595</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.9731752898266564E-9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <f>E4-E3</f>
-        <v>0.44948974278317788</v>
-      </c>
-      <c r="F5">
-        <f t="shared" ref="F5:I5" si="4">F4-F3</f>
-        <v>0.58113883008418976</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="4"/>
-        <v>0.58055246225798041</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
-        <v>0.56066017177982119</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="4"/>
-        <v>0.53808315196468592</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <f>E5/E3</f>
-        <v>0.22474487139158894</v>
-      </c>
-      <c r="F6">
-        <f t="shared" ref="F6:I6" si="5">F5/F3</f>
-        <v>0.58113883008418976</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="5"/>
-        <v>0.87082869338697066</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="5"/>
-        <v>1.1213203435596424</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="5"/>
-        <v>1.3452078799117146</v>
-      </c>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4.4269999999999996</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>9.5552732447545807E-6</v>
+      </c>
+      <c r="C6">
+        <f>15.269/16</f>
+        <v>0.95431250000000001</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <f>E4/2</f>
-        <v>1.2247448713915889</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:I7" si="6">F4/2</f>
-        <v>0.79056941504209488</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="6"/>
-        <v>0.62360956446232352</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="6"/>
-        <v>0.5303300858899106</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="6"/>
-        <v>0.46904157598234297</v>
-      </c>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <f>E2/2</f>
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <f>F2/2</f>
-        <v>0.25</v>
-      </c>
-      <c r="G8">
-        <f>G2/2</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="H8">
-        <f>H2/2</f>
-        <v>0.125</v>
-      </c>
-      <c r="I8">
-        <f>I2/2</f>
-        <v>0.1</v>
-      </c>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <f>SQRT(E2^2/4+E2^4*7/32+E2^6*75/128)</f>
-        <v>1.0269797953221864</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:I9" si="7">SQRT(F2^2/4+F2^4*7/32+F2^6*75/128)</f>
-        <v>0.29210811087249872</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="7"/>
-        <v>0.17686760643419505</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="7"/>
-        <v>0.12892844269190928</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="7"/>
-        <v>0.10191908555319755</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <f>E9-E8</f>
-        <v>0.52697979532218642</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ref="F10:I10" si="8">F9-F8</f>
-        <v>4.2108110872498716E-2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="8"/>
-        <v>1.0200939767528394E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="8"/>
-        <v>3.9284426919092841E-3</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="8"/>
-        <v>1.9190855531975443E-3</v>
-      </c>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <f>E10/E8</f>
-        <v>1.0539595906443728</v>
-      </c>
-      <c r="F11">
-        <f t="shared" ref="F11:I11" si="9">F10/F8</f>
-        <v>0.16843244348999487</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="9"/>
-        <v>6.1205638605170365E-2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="9"/>
-        <v>3.1427541535274273E-2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="9"/>
-        <v>1.9190855531975443E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E12">
-        <f>E9*2</f>
-        <v>2.0539595906443728</v>
-      </c>
-      <c r="F12">
-        <f t="shared" ref="F12:I12" si="10">F9*2</f>
-        <v>0.58421622174499743</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="10"/>
-        <v>0.3537352128683901</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="10"/>
-        <v>0.25785688538381857</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="10"/>
-        <v>0.2038381711063951</v>
-      </c>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve verification by math lib
</commit_message>
<xml_diff>
--- a/ToolBox/MomentumFactor.xlsx
+++ b/ToolBox/MomentumFactor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cheng\Documents\Proj\VarianceArithemtic\ToolBox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F174137-609A-43A3-AD8C-97B25519D75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855349C8-A94D-4812-A240-D334CE290403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7FD3F55C-C7F1-40E3-A8ED-B74ABB74A617}"/>
+    <workbookView xWindow="32415" yWindow="1950" windowWidth="17805" windowHeight="12870" xr2:uid="{7FD3F55C-C7F1-40E3-A8ED-B74ABB74A617}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="3" r:id="rId1"/>
@@ -22017,6 +22017,3451 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10742752266589212"/>
+          <c:y val="6.1745303530636002E-2"/>
+          <c:w val="0.85453126537602697"/>
+          <c:h val="0.86765479407313451"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Factor!$AF$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Factor!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Factor!$AF$2:$AF$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.97070909999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6728079999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.21016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59.086210000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>357.31169999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2360.252</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16551.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121090.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>913884.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7061878</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55582030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>443930200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3588146000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29288950000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>241060600000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1998010000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16660500000000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>139653100000000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1175983000000000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9942714000000000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.436571E+16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.181553E+17</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.130859E+18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.247516E+19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.5020620000000003E+20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.8708259999999999E+21</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.334655E+22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.877952E+23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.487939E+24</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.1540960000000002E+25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.867715E+26</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.621558E+27</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.409586E+28</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2267399999999999E+29</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.068767E+30</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.3208229999999996E+30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.1365370000000006E+31</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.1091039999999996E+32</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.2166720000000004E+33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.4406210000000004E+34</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.7650540000000003E+35</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1763680000000002E+36</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.662902E+37</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.214642E+38</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.8229770000000001E+39</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.4804849999999999E+40</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.1807629999999999E+41</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.9182810000000001E+42</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.688252E+43</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.486532E+44</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.3095260000000001E+45</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.154113E+46</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.017581E+47</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.9757040000000001E+47</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7.9202720000000006E+48</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.9916069999999995E+49</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.1740909999999997E+50</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.4540899999999997E+51</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8196909999999996E+52</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.2604799999999996E+53</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.7673429999999998E+54</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.3323030000000001E+55</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.9483690000000001E+56</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.609415E+57</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.310065E+58</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.0456019999999999E+59</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.8118840000000001E+60</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.6052710000000001E+61</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.4225629999999999E+62</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.260948E+63</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.117948E+64</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.9138510000000004E+64</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.7933940000000009E+65</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.8012010000000005E+66</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.9223660000000006E+67</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6.143747E+68</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.4537529999999997E+69</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.8421560000000001E+70</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.2999250000000002E+71</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.8190910000000003E+72</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.3926100000000001E+73</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.01426E+74</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.6785429999999998E+75</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.3805969999999999E+76</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.116122E+77</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.8813150000000002E+78</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.6728100000000001E+79</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.487628E+80</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.323133E+81</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.17699E+82</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.047129E+83</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.3171949999999997E+83</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.2913620000000006E+84</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>7.3794029999999997E+85</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.5685579999999998E+86</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.8475119999999997E+87</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.2062299999999999E+88</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>4.6358100000000001E+89</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4.1283539999999996E+90</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.6768530000000001E+91</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AECD-4D89-BBCE-A68C810B95CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Factor!$AP$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Factor!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Factor!$AP$2:$AP$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.99886600000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9794679999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.623250000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.977429999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>811.63130000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7805.2950000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83506.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>965198.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11810000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>150816100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1989955000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26934040000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>371992200000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5222047000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>74291480000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1068670000000000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.551625E+16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.27071E+17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.345664E+18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.958548E+19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.3867800000000007E+20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1053930000000001E+22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6607919999999999E+23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5041599999999998E+24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.7878850000000002E+25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.7462170000000003E+26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.7397549999999995E+27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3324340000000001E+29</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.035784E+30</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.1165819999999999E+31</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.7798769999999998E+32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.343192E+33</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.129869E+35</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.7409970000000001E+36</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.686274E+37</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.1499770000000001E+38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.4187209999999996E+39</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.9386279999999996E+40</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5404590000000001E+42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.3899739999999999E+43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.7113400000000001E+44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.7682039999999998E+45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>8.972269E+46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.3966800000000001E+48</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.1757389999999999E+49</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.3916909999999998E+50</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.290662E+51</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.2579900000000004E+52</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.2897230000000001E+54</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.015414E+55</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.151133E+56</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.929393E+57</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.7149739999999995E+58</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.208039E+60</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.8924480000000001E+61</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.9658950000000001E+62</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.6501689999999998E+63</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.2938319999999995E+64</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.144485E+66</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.796492E+67</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.8209510000000001E+68</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.4311379999999999E+69</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.9627200000000002E+70</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.094414E+72</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.720752E+73</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.706354E+74</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.2577099999999997E+75</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7002150000000004E+76</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0546749999999999E+78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.6605879999999999E+79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.6152609999999998E+80</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1197859999999998E+81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6.4913870000000005E+82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.0230589999999999E+84</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.6127270000000002E+85</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.5428189999999998E+86</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.010161E+87</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.3255329999999997E+88</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>9.9797360000000001E+89</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.574799E+91</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.4854970000000001E+92</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9235659999999998E+93</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.1947860000000002E+94</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>9.7824409999999995E+95</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.545047E+97</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.4406639999999999E+98</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.856065E+99</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.0932470000000002E+100</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.6298569999999999E+101</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.522144E+103</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.40633E+104</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.8046640000000001E+105</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.016417E+106</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.5152149999999997E+107</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.505071E+109</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.3809579999999999E+110</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.767052E+111</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.9608109999999997E+112</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.4332610000000004E+113</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.4930350000000001E+115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AECD-4D89-BBCE-A68C810B95CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Factor!$AZ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Factor!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Factor!$AZ$2:$AZ$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.9999846</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9995820000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.988619999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>936.38469999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10155.040000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128385.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1835046</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28927230</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>492903600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8933129000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>170015800000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3364241000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>68680670000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1437893000000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.072853E+16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.678877E+17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.472222E+19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2837609999999998E+20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.3980139999999998E+21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.681022E+23</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.8479859999999998E+24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.8649169999999992E+25</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.053755E+27</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.781512E+28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1180990000000001E+30</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6247440000000001E+31</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.1831420000000003E+32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.461153E+34</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.4627070000000004E+35</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.2272790000000002E+36</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.9593770000000001E+38</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.6764269999999999E+39</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1183260000000001E+41</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.6792450000000001E+42</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.4296370000000003E+43</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.5453839999999999E+45</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.719755E+46</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.9655410000000008E+47</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.163635E+49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.2275900000000001E+50</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.2644360000000001E+52</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.0615449999999998E+53</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.4200430000000005E+54</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.7999879999999999E+56</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.3702670000000003E+57</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0619420000000001E+59</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.5824339999999999E+60</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6.2845729999999996E+61</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.5304679999999999E+63</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7295769999999998E+64</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9.0942729999999991E+65</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.218893E+67</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.4169259999999999E+68</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.323141E+70</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.233596E+71</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.9064529999999996E+72</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.9341269999999999E+74</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.7335479999999997E+75</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1589889999999999E+77</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.8389280000000001E+78</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.9567340000000002E+79</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.705396E+81</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.1822279999999999E+82</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.025998E+84</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.5178880000000001E+85</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.1811810000000004E+86</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.517913E+88</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.7287009999999998E+89</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.1621859999999997E+90</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.2519929999999999E+92</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.5367810000000002E+93</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.3616509999999999E+95</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.3495679999999998E+96</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.2418130000000004E+97</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.028449E+99</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.9935550000000002E+100</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.229579E+102</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.028317E+103</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.4600419999999997E+104</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.838119E+106</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4.5299779999999999E+107</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.1166209999999999E+109</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.752963E+110</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.788559E+111</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.6743080000000001E+113</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.1302009999999997E+114</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.019022E+116</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.514605E+117</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.2062400000000003E+118</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.5319969999999999E+120</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.7822999999999999E+121</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.3394489999999995E+122</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.3064920000000001E+124</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.6970040000000001E+125</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.407355E+127</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.4771340000000001E+128</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.5920899999999996E+129</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.1234130000000001E+131</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5.2483980000000002E+132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AECD-4D89-BBCE-A68C810B95CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Factor!$BJ$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Factor!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Factor!$BJ$2:$BJ$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.99999990000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.999890000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>104.9958</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>944.84010000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10388.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>134896.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017728</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34095690</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>640413300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13182110000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>293591800000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6994317000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>176409400000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4668132000000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.285934E+17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.663313E+18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.073262E+20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2190389999999999E+21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8469409999999994E+22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.0626139999999999E+24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.6605639999999992E+25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.0841310000000001E+27</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.9481709999999995E+28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2375970000000002E+30</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0618520000000001E+32</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.5062520000000001E+33</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.164676E+35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.8891109999999997E+36</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3047390000000001E+38</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3955020000000003E+39</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.486339E+41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.0430239999999997E+42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.716282E+44</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.8571890000000001E+45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.0039469999999999E+47</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.8720500000000004E+48</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.3616019999999999E+50</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.1315659999999993E+51</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.804941E+53</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.6916330000000004E+54</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.3538359999999999E+56</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.1622819999999999E+58</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.0333249999999998E+59</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4013899999999999E+61</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.8748849999999999E+62</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6976470000000001E+64</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.9180560000000004E+65</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.0650630000000001E+67</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.2125040000000002E+68</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.521244E+70</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8.8206239999999995E+71</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.0883090000000003E+73</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.082085E+75</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.7940730000000001E+76</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.331185E+78</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.6735330000000002E+79</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.6417760000000001E+81</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.770747E+82</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.0294970000000002E+84</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.1412210000000001E+85</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.5140529999999999E+87</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.8549290000000001E+88</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.1202950000000002E+90</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.100014E+92</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.879582E+93</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.3688269999999999E+95</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8315050000000001E+96</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.7060040000000001E+98</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.0260849999999996E+99</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.1293270000000002E+101</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.5265530000000005E+102</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.661283E+104</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9.412881999999999E+105</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.3303190000000003E+107</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.178628E+109</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.1724430000000003E+110</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.477487E+112</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.2332570000000001E+113</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.8540960000000001E+115</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.5705370000000003E+116</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.3290269999999998E+118</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.2575259999999999E+119</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.9283589999999999E+121</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.038711E+123</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.6851739999999998E+124</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.3077119999999999E+126</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.641454E+127</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.6477140000000001E+129</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.8504950000000003E+130</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.0777080000000001E+132</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7.3799830000000004E+133</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.6218210000000001E+135</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3159129999999997E+136</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.3107069999999998E+138</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.176758E+140</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.1833369999999998E+141</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.4873949999999999E+143</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.289267E+144</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.8811750000000001E+146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AECD-4D89-BBCE-A68C810B95CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Factor!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(2n-1)!!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Factor!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Factor!$B$2:$B$101</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>945</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135135</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027025</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34459430</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>654729100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13749310000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>316234100000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7905854000000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>213458000000000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6190283000000000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.918988E+17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.33266E+18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2164310000000002E+20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.200795E+21</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.1983100000000002E+23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3113069999999999E+25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.6386200000000001E+26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5373789999999999E+28</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.1925680000000001E+30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.8435840000000002E+31</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.9802280000000001E+33</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.579521E+35</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.6873640000000005E+36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.9517980000000002E+38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9215609999999999E+40</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.7821519999999999E+42</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.122756E+44</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.2979120000000004E+45</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.8896010000000003E+47</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.373825E+49</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.395416E+51</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.748653E+53</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3114900000000001E+55</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0098469999999999E+57</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.9777939999999996E+58</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.4620129999999999E+60</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.3634709999999997E+62</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.5589500000000001E+64</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.9662869999999999E+66</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.5299950000000002E+68</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.2122959999999999E+70</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.987435E+72</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.8380629999999999E+74</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.752921E+76</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.725392E+78</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.7526459999999998E+80</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.8352249999999999E+82</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.976987E+84</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.1853760000000003E+86</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.4720599999999997E+88</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.8539860000000001E+90</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.3550039999999998E+92</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.008255E+94</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8596579999999999E+96</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.9729929999999996E+98</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8.4373219999999999E+100</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.037791E+103</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.2972380000000001E+105</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.647493E+107</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.1252649999999998E+109</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.784098E+111</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.70285E+113</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.9988480000000002E+115</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8484209999999999E+117</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.5193049999999997E+119</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.3422220000000001E+122</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.9193779999999999E+124</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.7830970000000003E+126</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.0911529999999998E+128</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6.0958179999999995E+130</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.2046860000000005E+132</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.408317E+135</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.1828910000000002E+137</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.4271390000000001E+139</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.4491510000000003E+141</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.7731339999999996E+143</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.4300210000000001E+146</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.359534E+148</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.9404220000000001E+150</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.6593139999999998E+152</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.1387429999999999E+155</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.970025E+157</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.4475430000000001E+159</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.1021520000000002E+161</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.092285E+164</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.9770359999999999E+166</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.6179760000000001E+168</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.6932559999999996E+170</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.251639E+173</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.365597E+175</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.5182909999999999E+177</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>8.7203019999999994E+179</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.7004590000000001E+182</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.349904E+184</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.6663090000000003E+186</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AECD-4D89-BBCE-A68C810B95CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="267875807"/>
+        <c:axId val="267881567"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="267875807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267881567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="267881567"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1000000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267875807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10780733785428621"/>
+          <c:y val="6.2913012448807634E-2"/>
+          <c:w val="0.10611218589851543"/>
+          <c:h val="0.25794485611998047"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -30696,6 +34141,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>110096</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E0520C4-2B3D-4DDF-AF09-DDF673165C5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -31649,8 +35132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69331D1-8607-4904-B05A-525081DDFA9E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="O60" sqref="O60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31665,7 +35148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5B3A00-F35E-4121-9A2D-44E8B51672C0}">
   <dimension ref="A1:T200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>